<commit_message>
corrigiendo valores del excel
</commit_message>
<xml_diff>
--- a/planillaZulliger.xlsx
+++ b/planillaZulliger.xlsx
@@ -7,7 +7,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja de datos" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -439,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,7 +474,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Determinantes</t>
+          <t>Det</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -490,7 +489,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Contenidos</t>
+          <t>Cont</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -510,16 +509,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>?</t>
@@ -537,7 +534,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>FM</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -545,14 +542,9 @@
           <t>?</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -572,49 +564,47 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>C',M</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>H,H</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -634,10 +624,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -661,7 +649,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>m</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -669,19 +657,9 @@
           <t>?</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>?</t>
+          <t>Fi</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -696,124 +674,143 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A5" t="n">
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>?</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>?</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2</t>
+          <t>?</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ad,Ad</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Hx</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>?</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A5:L5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>det</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>par</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>cont</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>pop</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
falta mergear filas en excel
</commit_message>
<xml_diff>
--- a/planillaZulliger.xlsx
+++ b/planillaZulliger.xlsx
@@ -534,10 +534,15 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>FM</t>
+          <t>C',FM</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>?</t>
         </is>
@@ -589,7 +594,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>C',M</t>
+          <t>m</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -599,12 +604,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>H,H</t>
+          <t>Fi</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -649,7 +654,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>m</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -657,9 +662,19 @@
           <t>?</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Fi</t>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>?</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -675,7 +690,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -697,14 +712,29 @@
           <t>?</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Ad,Ad</t>
+          <t>Ad</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>?</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -720,7 +750,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -742,7 +772,27 @@
           <t>?</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Hx</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
         <is>
           <t>?</t>
         </is>
@@ -760,7 +810,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -784,7 +834,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>?</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -792,13 +842,21 @@
           <t>?</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Hx</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
+          <t>Hd</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>?</t>

</xml_diff>

<commit_message>
fallas en contenidos y determinantes, número de lámina y carga a excel
</commit_message>
<xml_diff>
--- a/planillaZulliger.xlsx
+++ b/planillaZulliger.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,7 +534,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>C',FM,C',FM</t>
+          <t xml:space="preserve"> C', FM</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -549,12 +549,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>A,A</t>
+          <t xml:space="preserve"> A</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>??</t>
+          <t>Po1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -563,126 +563,6 @@
         </is>
       </c>
       <c r="L2" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>C',FM</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>C',FM</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
         <is>
           <t>?</t>
         </is>

</xml_diff>

<commit_message>
fallas en agregado a excel
</commit_message>
<xml_diff>
--- a/planillaZulliger.xlsx
+++ b/planillaZulliger.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A</t>
+          <t xml:space="preserve"> A Ad,</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -563,6 +563,126 @@
         </is>
       </c>
       <c r="L2" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> m, C</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fi Hx,</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> M, M</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> H H, Hd,</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Po3</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>?</t>
         </is>

</xml_diff>